<commit_message>
Update 29 mayo 2023
</commit_message>
<xml_diff>
--- a/bases/voto2021_v2.xlsx
+++ b/bases/voto2021_v2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Arturo/Documents/GitHub/arturomaldonado.github.io/bases/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71165AE6-5E8A-8A46-9DC1-5FAEDBC81164}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4590D017-6F25-7D44-AFF7-772ABA455069}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3380" yWindow="7140" windowWidth="25240" windowHeight="17020" xr2:uid="{723A9531-B34C-4361-B3F5-4DFC2977AD96}"/>
+    <workbookView xWindow="3380" yWindow="980" windowWidth="25240" windowHeight="17020" xr2:uid="{723A9531-B34C-4361-B3F5-4DFC2977AD96}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="4" r:id="rId1"/>
@@ -20,11 +20,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -116,9 +111,6 @@
     <t>IngresoMensual2020</t>
   </si>
   <si>
-    <t>Al menos 1 NBI</t>
-  </si>
-  <si>
     <t>SeguroSalud</t>
   </si>
   <si>
@@ -141,6 +133,9 @@
   </si>
   <si>
     <t>VotoVM_1</t>
+  </si>
+  <si>
+    <t>NBI1</t>
   </si>
 </sst>
 </file>
@@ -201,7 +196,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -210,7 +205,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
@@ -532,8 +526,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{898B44A7-E4C4-4F34-BDD4-A9EC79F71141}">
   <dimension ref="A1:L29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="144" zoomScaleNormal="144" workbookViewId="0">
-      <selection activeCell="L27" sqref="L27"/>
+    <sheetView tabSelected="1" zoomScale="144" zoomScaleNormal="144" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -543,37 +537,37 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" t="s">
         <v>32</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K1" t="s">
         <v>33</v>
       </c>
-      <c r="D1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G1" t="s">
-        <v>29</v>
-      </c>
-      <c r="H1" t="s">
-        <v>30</v>
-      </c>
-      <c r="I1" t="s">
-        <v>31</v>
-      </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>34</v>
-      </c>
-      <c r="K1" t="s">
-        <v>35</v>
-      </c>
-      <c r="L1" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
@@ -587,31 +581,31 @@
         <v>13.5</v>
       </c>
       <c r="D2">
+        <v>6.73</v>
+      </c>
+      <c r="E2">
         <v>704</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>34.6</v>
       </c>
-      <c r="F2" s="2">
+      <c r="G2" s="2">
         <v>30.172448510374494</v>
       </c>
-      <c r="G2" s="2">
+      <c r="H2" s="2">
         <v>89.907340725117109</v>
       </c>
-      <c r="H2" s="3">
+      <c r="I2" s="3">
         <v>17.899999999999999</v>
       </c>
-      <c r="I2" s="3">
+      <c r="J2" s="3">
         <v>8.0348132955024649</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>1.1399999999999999</v>
       </c>
-      <c r="K2">
+      <c r="L2">
         <v>0.73</v>
-      </c>
-      <c r="L2">
-        <v>6.73</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
@@ -625,31 +619,31 @@
         <v>14.3</v>
       </c>
       <c r="D3">
+        <v>8.43</v>
+      </c>
+      <c r="E3">
         <v>755</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>34.6</v>
       </c>
-      <c r="F3" s="2">
+      <c r="G3" s="2">
         <v>17.2014035176195</v>
       </c>
-      <c r="G3" s="2">
+      <c r="H3" s="2">
         <v>82.730621293742729</v>
       </c>
-      <c r="H3" s="3">
+      <c r="I3" s="3">
         <v>16.2</v>
       </c>
-      <c r="I3" s="3">
+      <c r="J3" s="3">
         <v>9.0116889602642782</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>3.25</v>
       </c>
-      <c r="K3">
+      <c r="L3">
         <v>4.8499999999999996</v>
-      </c>
-      <c r="L3">
-        <v>8.43</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
@@ -663,31 +657,31 @@
         <v>9.4</v>
       </c>
       <c r="D4">
+        <v>9.25</v>
+      </c>
+      <c r="E4">
         <v>697</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>34.6</v>
       </c>
-      <c r="F4" s="2">
+      <c r="G4" s="2">
         <v>11.348341993281853</v>
       </c>
-      <c r="G4" s="2">
+      <c r="H4" s="2">
         <v>90.072335826745601</v>
       </c>
-      <c r="H4" s="3">
+      <c r="I4" s="3">
         <v>16.100000000000001</v>
       </c>
-      <c r="I4" s="3">
+      <c r="J4" s="3">
         <v>12.630720874121621</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>0.1</v>
       </c>
-      <c r="K4">
+      <c r="L4">
         <v>4.58</v>
-      </c>
-      <c r="L4">
-        <v>9.25</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
@@ -701,31 +695,31 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="D5">
+        <v>6.95</v>
+      </c>
+      <c r="E5">
         <v>1028</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>19.5</v>
       </c>
-      <c r="F5" s="2">
+      <c r="G5" s="2">
         <v>10.59292185586947</v>
       </c>
-      <c r="G5" s="2">
+      <c r="H5" s="2">
         <v>66.931592380654763</v>
       </c>
-      <c r="H5" s="3">
+      <c r="I5" s="3">
         <v>6.1</v>
       </c>
-      <c r="I5" s="3">
+      <c r="J5" s="3">
         <v>3.1306865844505638</v>
       </c>
-      <c r="J5" s="5">
+      <c r="K5" s="4">
         <v>2.93</v>
       </c>
-      <c r="K5" s="5">
+      <c r="L5" s="4">
         <v>6.49</v>
-      </c>
-      <c r="L5">
-        <v>6.95</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
@@ -739,31 +733,31 @@
         <v>7.1</v>
       </c>
       <c r="D6">
+        <v>9.7799999999999994</v>
+      </c>
+      <c r="E6">
         <v>710</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>45.9</v>
       </c>
-      <c r="F6" s="2">
+      <c r="G6" s="2">
         <v>19.184791443420607</v>
       </c>
-      <c r="G6" s="2">
+      <c r="H6" s="2">
         <v>89.486362642321623</v>
       </c>
-      <c r="H6" s="3">
+      <c r="I6" s="3">
         <v>17.3</v>
       </c>
-      <c r="I6" s="3">
+      <c r="J6" s="3">
         <v>11.52833968628536</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <v>0.47</v>
       </c>
-      <c r="K6">
+      <c r="L6">
         <v>6.53</v>
-      </c>
-      <c r="L6">
-        <v>9.7799999999999994</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
@@ -777,31 +771,31 @@
         <v>10.6</v>
       </c>
       <c r="D7">
+        <v>5.75</v>
+      </c>
+      <c r="E7">
         <v>632</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>45.9</v>
       </c>
-      <c r="F7" s="2">
+      <c r="G7" s="2">
         <v>17.195311104060472</v>
       </c>
-      <c r="G7" s="2">
+      <c r="H7" s="2">
         <v>87.135896197031258</v>
       </c>
-      <c r="H7" s="3">
+      <c r="I7" s="3">
         <v>25.6</v>
       </c>
-      <c r="I7" s="3">
+      <c r="J7" s="3">
         <v>12.135443058681924</v>
       </c>
-      <c r="J7">
+      <c r="K7">
         <v>7.23</v>
       </c>
-      <c r="K7">
+      <c r="L7">
         <v>1.1399999999999999</v>
-      </c>
-      <c r="L7">
-        <v>5.75</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
@@ -815,31 +809,31 @@
         <v>15.2</v>
       </c>
       <c r="D8">
+        <v>7.28</v>
+      </c>
+      <c r="E8">
         <v>782</v>
       </c>
-      <c r="E8">
+      <c r="F8">
         <v>34.6</v>
       </c>
-      <c r="F8" s="2">
+      <c r="G8" s="2">
         <v>5.1148147268565145</v>
       </c>
-      <c r="G8" s="2">
+      <c r="H8" s="2">
         <v>77.536144744720815</v>
       </c>
-      <c r="H8" s="3">
+      <c r="I8" s="3">
         <v>3.8</v>
       </c>
-      <c r="I8" s="3">
+      <c r="J8" s="3">
         <v>1.8730342706563603</v>
       </c>
-      <c r="J8">
+      <c r="K8">
         <v>4.63</v>
       </c>
-      <c r="K8">
+      <c r="L8">
         <v>1.48</v>
-      </c>
-      <c r="L8">
-        <v>7.28</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
@@ -853,31 +847,31 @@
         <v>4.5</v>
       </c>
       <c r="D9">
+        <v>20.29</v>
+      </c>
+      <c r="E9">
         <v>651</v>
       </c>
-      <c r="E9">
+      <c r="F9">
         <v>34.6</v>
       </c>
-      <c r="F9" s="2">
+      <c r="G9" s="2">
         <v>13.546762877841028</v>
       </c>
-      <c r="G9" s="2">
+      <c r="H9" s="2">
         <v>82.259139894142436</v>
       </c>
-      <c r="H9" s="3">
+      <c r="I9" s="3">
         <v>14</v>
       </c>
-      <c r="I9" s="3">
+      <c r="J9" s="3">
         <v>9.8595313301411238</v>
       </c>
-      <c r="J9">
+      <c r="K9">
         <v>0.28000000000000003</v>
       </c>
-      <c r="K9">
+      <c r="L9">
         <v>12.08</v>
-      </c>
-      <c r="L9">
-        <v>20.29</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
@@ -891,31 +885,31 @@
         <v>5.7</v>
       </c>
       <c r="D10">
+        <v>6.85</v>
+      </c>
+      <c r="E10">
         <v>503</v>
       </c>
-      <c r="E10">
+      <c r="F10">
         <v>45.9</v>
       </c>
-      <c r="F10" s="2">
+      <c r="G10" s="2">
         <v>20.539754286553855</v>
       </c>
-      <c r="G10" s="2">
+      <c r="H10" s="2">
         <v>94.099666128861401</v>
       </c>
-      <c r="H10" s="3">
+      <c r="I10" s="3">
         <v>30.7</v>
       </c>
-      <c r="I10" s="3">
+      <c r="J10" s="3">
         <v>12.496497922113592</v>
       </c>
-      <c r="J10">
+      <c r="K10">
         <v>0.03</v>
       </c>
-      <c r="K10">
+      <c r="L10">
         <v>3.61</v>
-      </c>
-      <c r="L10">
-        <v>6.85</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
@@ -929,31 +923,31 @@
         <v>11.1</v>
       </c>
       <c r="D11">
+        <v>5.27</v>
+      </c>
+      <c r="E11">
         <v>652</v>
       </c>
-      <c r="E11">
+      <c r="F11">
         <v>45.9</v>
       </c>
-      <c r="F11" s="2">
+      <c r="G11" s="2">
         <v>23.84042724413349</v>
       </c>
-      <c r="G11" s="2">
+      <c r="H11" s="2">
         <v>85.798189696593354</v>
       </c>
-      <c r="H11" s="3">
+      <c r="I11" s="3">
         <v>19.399999999999999</v>
       </c>
-      <c r="I11" s="3">
+      <c r="J11" s="3">
         <v>13.569498007721405</v>
       </c>
-      <c r="J11">
+      <c r="K11">
         <v>1.52</v>
       </c>
-      <c r="K11">
+      <c r="L11">
         <v>4.0199999999999996</v>
-      </c>
-      <c r="L11">
-        <v>5.27</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
@@ -967,31 +961,31 @@
         <v>15.3</v>
       </c>
       <c r="D12">
+        <v>7.54</v>
+      </c>
+      <c r="E12">
         <v>1002</v>
       </c>
-      <c r="E12">
+      <c r="F12">
         <v>11.3</v>
       </c>
-      <c r="F12" s="2">
+      <c r="G12" s="2">
         <v>8.9634533478365466</v>
       </c>
-      <c r="G12" s="2">
+      <c r="H12" s="2">
         <v>71.14717465788388</v>
       </c>
-      <c r="H12" s="3">
+      <c r="I12" s="3">
         <v>5.5</v>
       </c>
-      <c r="I12" s="3">
+      <c r="J12" s="3">
         <v>2.3039358682706363</v>
       </c>
-      <c r="J12">
+      <c r="K12">
         <v>4.01</v>
       </c>
-      <c r="K12">
+      <c r="L12">
         <v>1.65</v>
-      </c>
-      <c r="L12">
-        <v>7.54</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
@@ -1005,31 +999,31 @@
         <v>13.9</v>
       </c>
       <c r="D13">
+        <v>9.11</v>
+      </c>
+      <c r="E13">
         <v>764</v>
       </c>
-      <c r="E13">
+      <c r="F13">
         <v>34.6</v>
       </c>
-      <c r="F13" s="2">
+      <c r="G13" s="2">
         <v>23.103275860209436</v>
       </c>
-      <c r="G13" s="2">
+      <c r="H13" s="2">
         <v>73.671151441163275</v>
       </c>
-      <c r="H13" s="3">
+      <c r="I13" s="3">
         <v>18.7</v>
       </c>
-      <c r="I13" s="3">
+      <c r="J13" s="3">
         <v>7.0204200884776906</v>
       </c>
-      <c r="J13">
+      <c r="K13">
         <v>0.53</v>
       </c>
-      <c r="K13">
+      <c r="L13">
         <v>6.39</v>
-      </c>
-      <c r="L13">
-        <v>9.11</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
@@ -1043,31 +1037,31 @@
         <v>16.8</v>
       </c>
       <c r="D14">
+        <v>4.78</v>
+      </c>
+      <c r="E14">
         <v>849</v>
       </c>
-      <c r="E14">
+      <c r="F14">
         <v>34.6</v>
       </c>
-      <c r="F14" s="2">
+      <c r="G14" s="2">
         <v>10.143241834688267</v>
       </c>
-      <c r="G14" s="2">
+      <c r="H14" s="2">
         <v>72.803145198883072</v>
       </c>
-      <c r="H14" s="3">
+      <c r="I14" s="3">
         <v>12.7</v>
       </c>
-      <c r="I14" s="3">
+      <c r="J14" s="3">
         <v>5.0900826938140131</v>
       </c>
-      <c r="J14">
+      <c r="K14">
         <v>12.31</v>
       </c>
-      <c r="K14">
+      <c r="L14">
         <v>0.73</v>
-      </c>
-      <c r="L14">
-        <v>4.78</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
@@ -1081,31 +1075,31 @@
         <v>21.4</v>
       </c>
       <c r="D15">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="E15">
         <v>879</v>
       </c>
-      <c r="E15">
+      <c r="F15">
         <v>19.5</v>
       </c>
-      <c r="F15" s="2">
+      <c r="G15" s="2">
         <v>10.237680257377169</v>
       </c>
-      <c r="G15" s="2">
+      <c r="H15" s="2">
         <v>78.61055639426597</v>
       </c>
-      <c r="H15" s="3">
+      <c r="I15" s="3">
         <v>11.2</v>
       </c>
-      <c r="I15" s="3">
+      <c r="J15" s="3">
         <v>5.2418786412068377</v>
       </c>
-      <c r="J15">
+      <c r="K15">
         <v>9.49</v>
       </c>
-      <c r="K15">
+      <c r="L15">
         <v>0.69</v>
-      </c>
-      <c r="L15">
-        <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
@@ -1119,31 +1113,31 @@
         <v>14.2</v>
       </c>
       <c r="D16">
+        <v>8.1300000000000008</v>
+      </c>
+      <c r="E16">
         <v>1022</v>
       </c>
-      <c r="E16">
+      <c r="F16">
         <v>28.6</v>
       </c>
-      <c r="F16" s="2">
+      <c r="G16" s="2">
         <v>9.4149583823864109</v>
       </c>
-      <c r="G16" s="2">
+      <c r="H16" s="2">
         <v>74.798336341721026</v>
       </c>
-      <c r="H16" s="3">
+      <c r="I16" s="3">
         <v>5</v>
       </c>
-      <c r="I16" s="3">
+      <c r="J16" s="3">
         <v>2.2978909167723534</v>
       </c>
-      <c r="J16">
+      <c r="K16">
         <v>26.64</v>
       </c>
-      <c r="K16">
+      <c r="L16">
         <v>22.5</v>
-      </c>
-      <c r="L16">
-        <v>8.1300000000000008</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
@@ -1157,31 +1151,31 @@
         <v>16.7</v>
       </c>
       <c r="D17">
+        <v>6.25</v>
+      </c>
+      <c r="E17">
         <v>628</v>
       </c>
-      <c r="E17">
+      <c r="F17">
         <v>34.6</v>
       </c>
-      <c r="F17" s="2">
+      <c r="G17" s="2">
         <v>52.425630527402205</v>
       </c>
-      <c r="G17" s="2">
+      <c r="H17" s="2">
         <v>86.837797397296484</v>
       </c>
-      <c r="H17" s="3">
+      <c r="I17" s="3">
         <v>23.7</v>
       </c>
-      <c r="I17" s="3">
+      <c r="J17" s="3">
         <v>6.4257112334430655</v>
       </c>
-      <c r="J17">
+      <c r="K17">
         <v>2.0499999999999998</v>
       </c>
-      <c r="K17">
+      <c r="L17">
         <v>1.18</v>
-      </c>
-      <c r="L17">
-        <v>6.25</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
@@ -1195,31 +1189,31 @@
         <v>11.3</v>
       </c>
       <c r="D18">
+        <v>6.77</v>
+      </c>
+      <c r="E18">
         <v>848</v>
       </c>
-      <c r="E18">
+      <c r="F18">
         <v>11.3</v>
       </c>
-      <c r="F18" s="2">
+      <c r="G18" s="2">
         <v>23.215076197710744</v>
       </c>
-      <c r="G18" s="2">
+      <c r="H18" s="2">
         <v>69.859792527025292</v>
       </c>
-      <c r="H18" s="3">
+      <c r="I18" s="3">
         <v>8.4</v>
       </c>
-      <c r="I18" s="3">
+      <c r="J18" s="3">
         <v>3.5204215160154266</v>
       </c>
-      <c r="J18">
+      <c r="K18">
         <v>0.34</v>
       </c>
-      <c r="K18">
+      <c r="L18">
         <v>0.71</v>
-      </c>
-      <c r="L18">
-        <v>6.77</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
@@ -1233,31 +1227,31 @@
         <v>4.7</v>
       </c>
       <c r="D19">
+        <v>7.34</v>
+      </c>
+      <c r="E19">
         <v>1218</v>
       </c>
-      <c r="E19">
+      <c r="F19">
         <v>19.5</v>
       </c>
-      <c r="F19" s="2">
+      <c r="G19" s="2">
         <v>10.96519941879308</v>
       </c>
-      <c r="G19" s="2">
+      <c r="H19" s="2">
         <v>80.750638573718277</v>
       </c>
-      <c r="H19" s="3">
+      <c r="I19" s="3">
         <v>2.5</v>
       </c>
-      <c r="I19" s="3">
+      <c r="J19" s="3">
         <v>4.3073255865818076</v>
       </c>
-      <c r="J19">
+      <c r="K19">
         <v>0.45</v>
       </c>
-      <c r="K19">
+      <c r="L19">
         <v>0.87</v>
-      </c>
-      <c r="L19">
-        <v>7.34</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
@@ -1271,31 +1265,31 @@
         <v>12.6</v>
       </c>
       <c r="D20">
+        <v>6.9</v>
+      </c>
+      <c r="E20">
         <v>594</v>
       </c>
-      <c r="E20">
+      <c r="F20">
         <v>45.9</v>
       </c>
-      <c r="F20" s="2">
+      <c r="G20" s="2">
         <v>29.896691812665964</v>
       </c>
-      <c r="G20" s="2">
+      <c r="H20" s="2">
         <v>84.963527982870772</v>
       </c>
-      <c r="H20" s="3">
+      <c r="I20" s="3">
         <v>16</v>
       </c>
-      <c r="I20" s="3">
+      <c r="J20" s="3">
         <v>5.9577198457307698</v>
       </c>
-      <c r="J20">
+      <c r="K20">
         <v>0.19</v>
       </c>
-      <c r="K20">
+      <c r="L20">
         <v>1.46</v>
-      </c>
-      <c r="L20">
-        <v>6.9</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
@@ -1309,31 +1303,31 @@
         <v>24.8</v>
       </c>
       <c r="D21">
+        <v>6.36</v>
+      </c>
+      <c r="E21">
         <v>757</v>
       </c>
-      <c r="E21">
+      <c r="F21">
         <v>34.6</v>
       </c>
-      <c r="F21" s="2">
+      <c r="G21" s="2">
         <v>22.313125989785103</v>
       </c>
-      <c r="G21" s="2">
+      <c r="H21" s="2">
         <v>78.929787835516436</v>
       </c>
-      <c r="H21" s="3">
+      <c r="I21" s="3">
         <v>13</v>
       </c>
-      <c r="I21" s="3">
+      <c r="J21" s="3">
         <v>7.1036912619080681</v>
       </c>
-      <c r="J21">
+      <c r="K21">
         <v>15.08</v>
       </c>
-      <c r="K21">
+      <c r="L21">
         <v>0.56000000000000005</v>
-      </c>
-      <c r="L21">
-        <v>6.36</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
@@ -1347,31 +1341,31 @@
         <v>2.8</v>
       </c>
       <c r="D22">
+        <v>5.77</v>
+      </c>
+      <c r="E22">
         <v>633</v>
       </c>
-      <c r="E22">
+      <c r="F22">
         <v>45.9</v>
       </c>
-      <c r="F22" s="2">
+      <c r="G22" s="2">
         <v>20.866659580720448</v>
       </c>
-      <c r="G22" s="2">
+      <c r="H22" s="2">
         <v>69.611562598420875</v>
       </c>
-      <c r="H22" s="3">
+      <c r="I22" s="3">
         <v>12.6</v>
       </c>
-      <c r="I22" s="3">
+      <c r="J22" s="3">
         <v>8.6342222488512963</v>
       </c>
-      <c r="J22">
+      <c r="K22">
         <v>0.05</v>
       </c>
-      <c r="K22">
+      <c r="L22">
         <v>14.33</v>
-      </c>
-      <c r="L22">
-        <v>5.77</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.2">
@@ -1385,31 +1379,31 @@
         <v>14.9</v>
       </c>
       <c r="D23">
+        <v>5.46</v>
+      </c>
+      <c r="E23">
         <v>740</v>
       </c>
-      <c r="E23">
+      <c r="F23">
         <v>28.6</v>
       </c>
-      <c r="F23" s="2">
+      <c r="G23" s="2">
         <v>29.054628622995558</v>
       </c>
-      <c r="G23" s="2">
+      <c r="H23" s="2">
         <v>83.570907538449433</v>
       </c>
-      <c r="H23" s="3">
+      <c r="I23" s="3">
         <v>11.5</v>
       </c>
-      <c r="I23" s="3">
+      <c r="J23" s="3">
         <v>7.3486763619471009</v>
       </c>
-      <c r="J23">
+      <c r="K23">
         <v>3.47</v>
       </c>
-      <c r="K23">
+      <c r="L23">
         <v>0.65</v>
-      </c>
-      <c r="L23">
-        <v>5.46</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
@@ -1423,31 +1417,31 @@
         <v>4.8</v>
       </c>
       <c r="D24">
+        <v>7.24</v>
+      </c>
+      <c r="E24">
         <v>879</v>
       </c>
-      <c r="E24">
+      <c r="F24">
         <v>28.6</v>
       </c>
-      <c r="F24" s="2">
+      <c r="G24" s="2">
         <v>7.481578600094438</v>
       </c>
-      <c r="G24" s="2">
+      <c r="H24" s="2">
         <v>60.268085009993129</v>
       </c>
-      <c r="H24" s="3">
+      <c r="I24" s="3">
         <v>2.4</v>
       </c>
-      <c r="I24" s="3">
+      <c r="J24" s="3">
         <v>3.2951192944739032</v>
       </c>
-      <c r="J24">
+      <c r="K24">
         <v>0.56000000000000005</v>
       </c>
-      <c r="K24">
+      <c r="L24">
         <v>1.81</v>
-      </c>
-      <c r="L24">
-        <v>7.24</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.2">
@@ -1461,31 +1455,31 @@
         <v>37.1</v>
       </c>
       <c r="D25">
+        <v>5.34</v>
+      </c>
+      <c r="E25">
         <v>835</v>
       </c>
-      <c r="E25">
+      <c r="F25">
         <v>34.6</v>
       </c>
-      <c r="F25" s="2">
+      <c r="G25" s="2">
         <v>20.739240139794141</v>
       </c>
-      <c r="G25" s="2">
+      <c r="H25" s="2">
         <v>84.184259969067924</v>
       </c>
-      <c r="H25" s="3">
+      <c r="I25" s="3">
         <v>7.5</v>
       </c>
-      <c r="I25" s="3">
+      <c r="J25" s="3">
         <v>3.4920291977893863</v>
       </c>
-      <c r="J25">
+      <c r="K25">
         <v>2.38</v>
       </c>
-      <c r="K25">
+      <c r="L25">
         <v>0.06</v>
-      </c>
-      <c r="L25">
-        <v>5.34</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.2">
@@ -1499,36 +1493,35 @@
         <v>21.5</v>
       </c>
       <c r="D26">
+        <v>8.01</v>
+      </c>
+      <c r="E26">
         <v>682</v>
       </c>
-      <c r="E26">
+      <c r="F26">
         <v>28.6</v>
       </c>
-      <c r="F26" s="2">
+      <c r="G26" s="2">
         <v>43.44754261988696</v>
       </c>
-      <c r="G26" s="2">
+      <c r="H26" s="2">
         <v>76.138673468440288</v>
       </c>
-      <c r="H26" s="3">
+      <c r="I26" s="3">
         <v>17.7</v>
       </c>
-      <c r="I26" s="3">
+      <c r="J26" s="3">
         <v>4.7424988920022209</v>
       </c>
-      <c r="J26">
+      <c r="K26">
         <v>0.91</v>
       </c>
-      <c r="K26">
+      <c r="L26">
         <v>0.93</v>
       </c>
-      <c r="L26">
-        <v>8.01</v>
-      </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="F29" s="1"/>
-      <c r="H29" s="4"/>
+      <c r="G29" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>